<commit_message>
object are now getting picture taken of them and are getting shown in the object menu
</commit_message>
<xml_diff>
--- a/sprintPlan.xlsx
+++ b/sprintPlan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20348"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UniversityStuff\FINAL YEAR\comp3000\comp3000\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oclark1\Desktop\comp3000\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6AF4DA-1941-4740-A041-68B3D3F3935B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E81A24-CD31-4DFA-B7F6-6CC258681CB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15750" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -88,7 +88,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,13 +110,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -131,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -143,6 +156,8 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,7 +441,7 @@
   <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,6 +599,7 @@
       <c r="C4" t="s">
         <v>16</v>
       </c>
+      <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
@@ -591,6 +607,7 @@
       <c r="C5" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -598,6 +615,7 @@
       <c r="C6" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>

</xml_diff>

<commit_message>
added more to sprint plan dotnet changed file to be pickedup again
</commit_message>
<xml_diff>
--- a/sprintPlan.xlsx
+++ b/sprintPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oclark1\Desktop\comp3000\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E81A24-CD31-4DFA-B7F6-6CC258681CB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A55673-C53A-4118-9DEA-C672ED131BBD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15750" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -75,20 +75,47 @@
     <t>TASK NAMES</t>
   </si>
   <si>
-    <t>movability around 3d scene</t>
-  </si>
-  <si>
     <t>object Crud (creation deletetion)</t>
   </si>
   <si>
     <t>object Crud (viewing, updateing)</t>
+  </si>
+  <si>
+    <t>import yaml</t>
+  </si>
+  <si>
+    <t>export yaml</t>
+  </si>
+  <si>
+    <t>movability around 3d scene(map panning, map zooming)</t>
+  </si>
+  <si>
+    <t>demonstrate cooperation</t>
+  </si>
+  <si>
+    <t>create level using level editor</t>
+  </si>
+  <si>
+    <t>buffer</t>
+  </si>
+  <si>
+    <t>poster and description</t>
+  </si>
+  <si>
+    <t>fix bugs</t>
+  </si>
+  <si>
+    <t>added tasks</t>
+  </si>
+  <si>
+    <t>user testing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,13 +139,27 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="9"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -127,8 +168,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -141,10 +191,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -156,10 +209,14 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -438,17 +495,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.140625" customWidth="1"/>
+    <col min="3" max="3" width="54.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="6" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
@@ -548,6 +605,9 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
       <c r="C3" t="s">
         <v>15</v>
       </c>
@@ -597,66 +657,108 @@
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="6"/>
+        <v>17</v>
+      </c>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="5"/>
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L12" s="5"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M13" s="5"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C15" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C16" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>